<commit_message>
May extra edits 3
May extra edits 3
</commit_message>
<xml_diff>
--- a/7.2_Alternative_fouling_approach/7.2_Input_PFHpA.xlsx
+++ b/7.2_Alternative_fouling_approach/7.2_Input_PFHpA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Activated-Carbon-Modelling\1USEPA_PSDM\9PSDM_Fouling_alternative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Modelling-activated-carbon\7.2_Alternative_fouling_approach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0DEF3-07FE-4B85-AF02-52E493FB942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5994C2FA-97BD-4D84-B396-F4B408D7B6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13F7DD-731C-403E-ACEA-F853111BA809}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401BCFB4-DB77-4CE9-BB3A-E676947AF423}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>50000</v>
+        <v>0.04</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -1020,10 +1020,10 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="C3">
-        <v>50000</v>
+        <v>0.04</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -1048,7 +1048,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1611,61 +1611,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3E377063FFE5489A04E78E6AF321F7" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d56b0910c09b2f28088e837fc8a4b1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns4="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns6="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xmlns:ns7="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c38d2d5698dbedce593845e142ad0a0f" ns1:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2122,44 +2067,62 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D265CA-67CD-4AD3-99A3-30810910E78A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,4 +2143,41 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>